<commit_message>
Más grabaciones y distinción de salidas en rotondas
</commit_message>
<xml_diff>
--- a/dataset_excel/salida_rotonda_train.xlsx
+++ b/dataset_excel/salida_rotonda_train.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,50 +446,55 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>salida</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>throttle</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>steer</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>brake</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>light_state</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>hand_brake</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>reverse</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>speed</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>loc_x</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>loc_y</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>loc_z</t>
         </is>
@@ -507,35 +512,38 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.8500000238418579</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E2" t="n">
         <v>-0.4542153179645538</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
       <c r="H2" t="b">
         <v>0</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
         <v>27</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>24.91235733032227</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>10.03256797790527</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.001901950803585351</v>
       </c>
     </row>
@@ -551,35 +559,38 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.8500000238418579</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E3" t="n">
         <v>-0.518277645111084</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
       <c r="H3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
         <v>31</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>33.09413146972656</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>9.004858016967773</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.001762561732903123</v>
       </c>
     </row>
@@ -595,35 +606,38 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.8500000238418579</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E4" t="n">
         <v>-0.800000011920929</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
         <v>46</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>27.32585144042969</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>9.385771751403809</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>0.001726093236356974</v>
       </c>
     </row>
@@ -639,35 +653,38 @@
         </is>
       </c>
       <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.6211206316947937</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>0.3019987940788269</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
       <c r="H5" t="b">
         <v>0</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
         <v>47</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>30.31264114379883</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>8.58956241607666</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>0.001791248330846429</v>
       </c>
     </row>
@@ -683,35 +700,38 @@
         </is>
       </c>
       <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
         <v>0.650823175907135</v>
       </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
         <v>53</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>44.82271957397461</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>8.901202201843262</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>0.001715145073831081</v>
       </c>
     </row>
@@ -727,35 +747,38 @@
         </is>
       </c>
       <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
         <v>0.3998300433158875</v>
       </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
         <v>44</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>31.67047309875488</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>7.207676410675049</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>0.001967143965885043</v>
       </c>
     </row>
@@ -771,35 +794,38 @@
         </is>
       </c>
       <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
         <v>0.5461015701293945</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>-0.03338327631354332</v>
       </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
       <c r="H8" t="b">
         <v>0</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
         <v>43</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>40.15504455566406</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>8.797562599182129</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>0.001823291764594615</v>
       </c>
     </row>
@@ -815,35 +841,38 @@
         </is>
       </c>
       <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
         <v>0.3324174284934998</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>0.2627202868461609</v>
       </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
       <c r="H9" t="b">
         <v>0</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
         <v>32</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>23.51803588867188</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>8.809623718261719</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>0.002005825052037835</v>
       </c>
     </row>
@@ -859,35 +888,38 @@
         </is>
       </c>
       <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" t="n">
         <v>0.3543706238269806</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>0.06294164806604385</v>
       </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
       <c r="H10" t="b">
         <v>0</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
         <v>31</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>28.1052188873291</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>8.074143409729004</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>0.001942501054145396</v>
       </c>
     </row>
@@ -903,35 +935,38 @@
         </is>
       </c>
       <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
         <v>0.3543706238269806</v>
       </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
       <c r="H11" t="b">
         <v>0</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
         <v>30</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>31.62388610839844</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>7.940271854400635</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>0.00187566748354584</v>
       </c>
     </row>
@@ -947,35 +982,38 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.8500000238418579</v>
+        <v>3</v>
       </c>
       <c r="D12" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E12" t="n">
         <v>-0.800000011920929</v>
       </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
         <v>37</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>22.40671539306641</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>9.276981353759766</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>0.001868266961537302</v>
       </c>
     </row>
@@ -991,35 +1029,38 @@
         </is>
       </c>
       <c r="C13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" t="n">
         <v>0.4076186418533325</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>0.04804281145334244</v>
       </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
       <c r="H13" t="b">
         <v>0</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
         <v>36</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>28.2258129119873</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>7.930490970611572</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>0.00190961838234216</v>
       </c>
     </row>
@@ -1035,35 +1076,38 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.8500000238418579</v>
+        <v>3</v>
       </c>
       <c r="D14" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E14" t="n">
         <v>-0.02320455200970173</v>
       </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
       <c r="H14" t="b">
         <v>0</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
         <v>36</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>38.07754898071289</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>7.607615947723389</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>0.001825466169975698</v>
       </c>
     </row>
@@ -1079,35 +1123,38 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.8500000238418579</v>
+        <v>3</v>
       </c>
       <c r="D15" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E15" t="n">
         <v>-0.800000011920929</v>
       </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
       <c r="H15" t="b">
         <v>0</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
         <v>54</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>21.37916374206543</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>11.58283138275146</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>0.001752643496729434</v>
       </c>
     </row>
@@ -1123,35 +1170,38 @@
         </is>
       </c>
       <c r="C16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" t="n">
         <v>0.6162576675415039</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>0.1177174374461174</v>
       </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
       <c r="H16" t="b">
         <v>0</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
         <v>55</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>24.19950675964355</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>10.11562538146973</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
         <v>0.001801509759388864</v>
       </c>
     </row>
@@ -1167,35 +1217,38 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.8500000238418579</v>
+        <v>3</v>
       </c>
       <c r="D17" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E17" t="n">
         <v>-0.1545484960079193</v>
       </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
       <c r="H17" t="b">
         <v>0</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
         <v>56</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>34.89767074584961</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>7.92012882232666</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>0.001765804248861969</v>
       </c>
     </row>
@@ -1211,35 +1264,38 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.8500000238418579</v>
+        <v>3</v>
       </c>
       <c r="D18" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E18" t="n">
         <v>-0.1846833825111389</v>
       </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G18" t="b">
-        <v>0</v>
-      </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
         <v>58</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>43.95557403564453</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>8.045056343078613</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>0.001764697954058647</v>
       </c>
     </row>
@@ -1255,35 +1311,38 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.8500000238418579</v>
+        <v>3</v>
       </c>
       <c r="D19" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E19" t="n">
         <v>-0.02547265589237213</v>
       </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
       <c r="H19" t="b">
         <v>0</v>
       </c>
-      <c r="I19" t="n">
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
         <v>45</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>29.83609771728516</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>7.658502101898193</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
         <v>0.001762676169164479</v>
       </c>
     </row>
@@ -1299,564 +1358,603 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.8500000238418579</v>
+        <v>3</v>
       </c>
       <c r="D20" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E20" t="n">
         <v>0.03566714003682137</v>
       </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G20" t="b">
-        <v>0</v>
-      </c>
       <c r="H20" t="b">
         <v>0</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
         <v>49</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>43.06849670410156</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>7.255053520202637</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>0.001767292036674917</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>sigo recto</t>
+          <t>quito intermitente</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>STR</t>
+          <t>BLK-OFF</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.8500000238418579</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.372218132019043</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="inlineStr">
+        <v>-0.800000011920929</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G21" t="b">
-        <v>0</v>
-      </c>
       <c r="H21" t="b">
         <v>0</v>
       </c>
-      <c r="I21" t="n">
-        <v>67</v>
+      <c r="I21" t="b">
+        <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>16.8786449432373</v>
+        <v>37</v>
       </c>
       <c r="K21" t="n">
-        <v>10.18427085876465</v>
+        <v>-24.84807586669922</v>
       </c>
       <c r="L21" t="n">
-        <v>0.001386318122968078</v>
+        <v>-8.928755760192871</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.001759853330440819</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>acelero</t>
+          <t>atención coche</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>T-ON</t>
+          <t>CAR-NR</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.8500000238418579</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.6499999761581421</v>
+        <v>0.4764819741249084</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Right_Blinker</t>
-        </is>
-      </c>
-      <c r="G22" t="b">
-        <v>0</v>
+        <v>0.1387574821710587</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
       </c>
       <c r="H22" t="b">
         <v>0</v>
       </c>
-      <c r="I22" t="n">
-        <v>37</v>
+      <c r="I22" t="b">
+        <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>29.69099998474121</v>
+        <v>40</v>
       </c>
       <c r="K22" t="n">
-        <v>6.980615615844727</v>
+        <v>-35.09615707397461</v>
       </c>
       <c r="L22" t="n">
-        <v>0.001725253998301923</v>
+        <v>-4.425873279571533</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.001817073789425194</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>quito intermitente</t>
+          <t>freno</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BLK-OFF</t>
+          <t>B-ON</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.8500000238418579</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.5597079992294312</v>
+        <v>0.2360807955265045</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Right_Blinker</t>
-        </is>
-      </c>
-      <c r="G23" t="b">
-        <v>0</v>
+        <v>0.02397390082478523</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
       </c>
       <c r="H23" t="b">
         <v>0</v>
       </c>
-      <c r="I23" t="n">
-        <v>41</v>
+      <c r="I23" t="b">
+        <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>34.9161262512207</v>
+        <v>39</v>
       </c>
       <c r="K23" t="n">
-        <v>6.924717426300049</v>
+        <v>-41.02838897705078</v>
       </c>
       <c r="L23" t="n">
-        <v>0.001711521064862609</v>
+        <v>-3.736086368560791</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.001877002650871873</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>recto</t>
+          <t>quito intermitente</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>STR</t>
+          <t>BLK-OFF</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.8500000238418579</v>
+        <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.4999999701976776</v>
+        <v>0.4977049827575684</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-      <c r="G24" t="b">
-        <v>0</v>
+        <v>0.02797854132950306</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
       </c>
       <c r="H24" t="b">
         <v>0</v>
       </c>
-      <c r="I24" t="n">
-        <v>47</v>
+      <c r="I24" t="b">
+        <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>47.68802642822266</v>
+        <v>24</v>
       </c>
       <c r="K24" t="n">
-        <v>6.853055477142334</v>
+        <v>-10.99576377868652</v>
       </c>
       <c r="L24" t="n">
-        <v>0.001735629979521036</v>
+        <v>29.38389015197754</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.001745243091136217</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>acelero</t>
+          <t>mantengo acelerador</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>T-ON</t>
+          <t>T-HOLD</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.4934229850769043</v>
+        <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>0.1172990351915359</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Right_Blinker</t>
-        </is>
-      </c>
-      <c r="G25" t="b">
-        <v>0</v>
+        <v>-0.1432014256715775</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
       </c>
       <c r="H25" t="b">
         <v>0</v>
       </c>
-      <c r="I25" t="n">
-        <v>40</v>
+      <c r="I25" t="b">
+        <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>27.99835968017578</v>
+        <v>27</v>
       </c>
       <c r="K25" t="n">
-        <v>6.790670394897461</v>
+        <v>-10.85231876373291</v>
       </c>
       <c r="L25" t="n">
-        <v>0.001861286116763949</v>
+        <v>33.90761566162109</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.001745738903991878</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>quito intermitente</t>
+          <t>recto</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BLK-OFF</t>
+          <t>STR</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.4934229850769043</v>
+        <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Right_Blinker</t>
-        </is>
-      </c>
-      <c r="G26" t="b">
-        <v>0</v>
+        <v>-0.1018086075782776</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
       </c>
       <c r="H26" t="b">
         <v>0</v>
       </c>
-      <c r="I26" t="n">
-        <v>41</v>
+      <c r="I26" t="b">
+        <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>34.09680938720703</v>
+        <v>32</v>
       </c>
       <c r="K26" t="n">
-        <v>6.877932071685791</v>
+        <v>-10.70899295806885</v>
       </c>
       <c r="L26" t="n">
-        <v>0.001808452536351979</v>
+        <v>42.02705001831055</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.001745700836181641</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>recto</t>
+          <t>atención coche</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>STR</t>
+          <t>CAR-NR</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.8500000238418579</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.01935414783656597</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-      <c r="G27" t="b">
-        <v>0</v>
+        <v>-0.800000011920929</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
       </c>
       <c r="H27" t="b">
         <v>0</v>
       </c>
-      <c r="I27" t="n">
-        <v>42</v>
+      <c r="I27" t="b">
+        <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>43.85362243652344</v>
+        <v>37</v>
       </c>
       <c r="K27" t="n">
-        <v>7.178617477416992</v>
+        <v>-27.89566040039062</v>
       </c>
       <c r="L27" t="n">
-        <v>0.00181127549149096</v>
+        <v>-6.109109878540039</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.002020816784352064</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>quito intermitente</t>
+          <t>freno</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BLK-OFF</t>
+          <t>B-ON</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.4598324596881866</v>
+        <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>0.1650571972131729</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Right_Blinker</t>
-        </is>
-      </c>
-      <c r="G28" t="b">
-        <v>0</v>
+        <v>0.1275806128978729</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
       </c>
       <c r="H28" t="b">
         <v>0</v>
       </c>
-      <c r="I28" t="n">
-        <v>39</v>
+      <c r="I28" t="b">
+        <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>18.47971343994141</v>
+        <v>28</v>
       </c>
       <c r="K28" t="n">
-        <v>10.91950702667236</v>
+        <v>-36.70010757446289</v>
       </c>
       <c r="L28" t="n">
-        <v>0.001840763026848435</v>
+        <v>-3.941839456558228</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.002097530290484428</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>acelero</t>
+          <t>quito intermitente</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>T-ON</t>
+          <t>BLK-OFF</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.5326606631278992</v>
+        <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>0.02709723822772503</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" t="inlineStr">
+        <v>-0.800000011920929</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>Right_Blinker</t>
         </is>
       </c>
-      <c r="G29" t="b">
-        <v>0</v>
-      </c>
       <c r="H29" t="b">
         <v>0</v>
       </c>
-      <c r="I29" t="n">
-        <v>40</v>
+      <c r="I29" t="b">
+        <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>33.49202346801758</v>
+        <v>28</v>
       </c>
       <c r="K29" t="n">
-        <v>7.559193134307861</v>
+        <v>-11.0563497543335</v>
       </c>
       <c r="L29" t="n">
-        <v>0.001791133894585073</v>
+        <v>21.55831527709961</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.001751613570377231</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>recto</t>
+          <t>mantengo acelerador</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>STR</t>
+          <t>T-HOLD</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.8500000238418579</v>
+        <v>2</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.800000011920929</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" t="inlineStr">
+        <v>0.08813728392124176</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G30" t="b">
-        <v>0</v>
-      </c>
       <c r="H30" t="b">
         <v>0</v>
       </c>
-      <c r="I30" t="n">
-        <v>42</v>
+      <c r="I30" t="b">
+        <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>41.42177581787109</v>
+        <v>35</v>
       </c>
       <c r="K30" t="n">
-        <v>7.813515663146973</v>
+        <v>-9.771036148071289</v>
       </c>
       <c r="L30" t="n">
-        <v>0.001774883246980608</v>
+        <v>33.86393356323242</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.001746501890011132</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>quito intermitente</t>
+          <t>recto</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BLK-OFF</t>
+          <t>STR</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.26939657330513</v>
+        <v>2</v>
       </c>
       <c r="D31" t="n">
-        <v>0.2071176022291183</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Right_Blinker</t>
-        </is>
-      </c>
-      <c r="G31" t="b">
-        <v>0</v>
+        <v>0.03430747240781784</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
       </c>
       <c r="H31" t="b">
         <v>0</v>
       </c>
-      <c r="I31" t="n">
-        <v>43</v>
+      <c r="I31" t="b">
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>16.82260131835938</v>
+        <v>39</v>
       </c>
       <c r="K31" t="n">
-        <v>11.96101856231689</v>
+        <v>-9.842405319213867</v>
       </c>
       <c r="L31" t="n">
-        <v>0.002188548911362886</v>
+        <v>43.46834564208984</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.001763553591445088</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>acelero</t>
+          <t>mantengo acelerador</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>T-ON</t>
+          <t>T-HOLD</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.8500000238418579</v>
+        <v>4</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.3766342997550964</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-      <c r="G32" t="b">
-        <v>0</v>
+        <v>-0.800000011920929</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
       </c>
       <c r="H32" t="b">
         <v>0</v>
       </c>
-      <c r="I32" t="n">
-        <v>47</v>
+      <c r="I32" t="b">
+        <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>29.1521167755127</v>
+        <v>46</v>
       </c>
       <c r="K32" t="n">
-        <v>8.126897811889648</v>
+        <v>7.927767753601074</v>
       </c>
       <c r="L32" t="n">
-        <v>0.001644763862714171</v>
+        <v>-39.88853073120117</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.001673030783422291</v>
       </c>
     </row>
     <row r="33">
@@ -1871,36 +1969,1590 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.8500000238418579</v>
+        <v>4</v>
       </c>
       <c r="D33" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-0.7349636554718018</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>51</v>
+      </c>
+      <c r="K33" t="n">
+        <v>8.362979888916016</v>
+      </c>
+      <c r="L33" t="n">
+        <v>-48.82992553710938</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.001690769102424383</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>quito intermitente</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>BLK-OFF</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.26939657330513</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>51</v>
+      </c>
+      <c r="K34" t="n">
+        <v>-9.693531036376953</v>
+      </c>
+      <c r="L34" t="n">
+        <v>38.90052795410156</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.001776714227162302</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>mantengo acelerador</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>T-HOLD</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.1484721601009369</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>46</v>
+      </c>
+      <c r="K35" t="n">
+        <v>-9.810933113098145</v>
+      </c>
+      <c r="L35" t="n">
+        <v>45.78223419189453</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.002048778580501676</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>recto</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>STR</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-0.0256773829460144</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>36</v>
+      </c>
+      <c r="K36" t="n">
+        <v>-9.969786643981934</v>
+      </c>
+      <c r="L36" t="n">
+        <v>54.86038970947266</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.002055454300716519</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>quito intermitente</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>BLK-OFF</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>3</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-0.02605433948338032</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>34</v>
+      </c>
+      <c r="K37" t="n">
+        <v>27.06857299804688</v>
+      </c>
+      <c r="L37" t="n">
+        <v>7.770931243896484</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.001779308309778571</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>mantengo acelerador</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>T-HOLD</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>3</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.6066043972969055</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.01658904366195202</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>39</v>
+      </c>
+      <c r="K38" t="n">
+        <v>33.70355987548828</v>
+      </c>
+      <c r="L38" t="n">
+        <v>7.393404483795166</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.001693363185040653</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>recto</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>STR</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>3</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.6066043972969055</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>44</v>
+      </c>
+      <c r="K39" t="n">
+        <v>42.29274368286133</v>
+      </c>
+      <c r="L39" t="n">
+        <v>7.231575965881348</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.001709270407445729</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>sigo recto</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>STR</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>3</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-0.372218132019043</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>67</v>
+      </c>
+      <c r="K40" t="n">
+        <v>16.8786449432373</v>
+      </c>
+      <c r="L40" t="n">
+        <v>10.18427085876465</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.001386318122968078</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>quito intermitente</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>BLK-OFF</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>2</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.06877923011779785</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>36</v>
+      </c>
+      <c r="K41" t="n">
+        <v>-11.30509376525879</v>
+      </c>
+      <c r="L41" t="n">
+        <v>27.93583488464355</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.002132701920345426</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>acelero</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>T-ON</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>2</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-0.1853130608797073</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>25</v>
+      </c>
+      <c r="K42" t="n">
+        <v>-10.99330139160156</v>
+      </c>
+      <c r="L42" t="n">
+        <v>37.91963958740234</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0.001922359457239509</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>recto</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>STR</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>2</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-0.224352702498436</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>33</v>
+      </c>
+      <c r="K43" t="n">
+        <v>-10.95111656188965</v>
+      </c>
+      <c r="L43" t="n">
+        <v>44.02573776245117</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0.001574191963300109</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>acelero</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>T-ON</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>3</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-0.6499999761581421</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>37</v>
+      </c>
+      <c r="K44" t="n">
+        <v>29.69099998474121</v>
+      </c>
+      <c r="L44" t="n">
+        <v>6.980615615844727</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0.001725253998301923</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>quito intermitente</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BLK-OFF</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>3</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-0.5597079992294312</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>41</v>
+      </c>
+      <c r="K45" t="n">
+        <v>34.9161262512207</v>
+      </c>
+      <c r="L45" t="n">
+        <v>6.924717426300049</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0.001711521064862609</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>recto</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>STR</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>3</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-0.4999999701976776</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>47</v>
+      </c>
+      <c r="K46" t="n">
+        <v>47.68802642822266</v>
+      </c>
+      <c r="L46" t="n">
+        <v>6.853055477142334</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0.001735629979521036</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>acelero</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>T-ON</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>3</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.4934229850769043</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.1172990351915359</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>40</v>
+      </c>
+      <c r="K47" t="n">
+        <v>27.99835968017578</v>
+      </c>
+      <c r="L47" t="n">
+        <v>6.790670394897461</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0.001861286116763949</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>quito intermitente</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>BLK-OFF</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>3</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.4934229850769043</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" t="b">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>41</v>
+      </c>
+      <c r="K48" t="n">
+        <v>34.09680938720703</v>
+      </c>
+      <c r="L48" t="n">
+        <v>6.877932071685791</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0.001808452536351979</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>recto</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>STR</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>3</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-0.01935414783656597</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>42</v>
+      </c>
+      <c r="K49" t="n">
+        <v>43.85362243652344</v>
+      </c>
+      <c r="L49" t="n">
+        <v>7.178617477416992</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.00181127549149096</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>quito intermitente</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>BLK-OFF</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>3</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.4598324596881866</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.1650571972131729</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>39</v>
+      </c>
+      <c r="K50" t="n">
+        <v>18.47971343994141</v>
+      </c>
+      <c r="L50" t="n">
+        <v>10.91950702667236</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.001840763026848435</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>acelero</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>T-ON</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>3</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.5326606631278992</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.02709723822772503</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>40</v>
+      </c>
+      <c r="K51" t="n">
+        <v>33.49202346801758</v>
+      </c>
+      <c r="L51" t="n">
+        <v>7.559193134307861</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0.001791133894585073</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>recto</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>STR</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>3</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-0.800000011920929</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>42</v>
+      </c>
+      <c r="K52" t="n">
+        <v>41.42177581787109</v>
+      </c>
+      <c r="L52" t="n">
+        <v>7.813515663146973</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.001774883246980608</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>quito intermitente</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>BLK-OFF</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>3</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.26939657330513</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.2071176022291183</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" t="b">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>43</v>
+      </c>
+      <c r="K53" t="n">
+        <v>16.82260131835938</v>
+      </c>
+      <c r="L53" t="n">
+        <v>11.96101856231689</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.002188548911362886</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>acelero</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>T-ON</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>3</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-0.3766342997550964</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>47</v>
+      </c>
+      <c r="K54" t="n">
+        <v>29.1521167755127</v>
+      </c>
+      <c r="L54" t="n">
+        <v>8.126897811889648</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.001644763862714171</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>recto</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>STR</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>3</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E55" t="n">
         <v>-0.34540194272995</v>
       </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="inlineStr">
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G33" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" t="n">
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
         <v>53</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K55" t="n">
         <v>36.71184158325195</v>
       </c>
-      <c r="K33" t="n">
+      <c r="L55" t="n">
         <v>8.436331748962402</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M55" t="n">
         <v>0.001615505199879408</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>quito intermitente</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>BLK-OFF</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>2</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-0.2768785953521729</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="b">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>32</v>
+      </c>
+      <c r="K56" t="n">
+        <v>-14.99718856811523</v>
+      </c>
+      <c r="L56" t="n">
+        <v>13.28381156921387</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0.001328182173892856</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>mantengo acelerador</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>T-HOLD</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>2</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.01452135387808084</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H57" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" t="b">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>66</v>
+      </c>
+      <c r="K57" t="n">
+        <v>-10.91675662994385</v>
+      </c>
+      <c r="L57" t="n">
+        <v>32.65631866455078</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0.001369495410472155</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>recto</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>STR</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>2</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H58" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" t="b">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>75</v>
+      </c>
+      <c r="K58" t="n">
+        <v>-10.72840785980225</v>
+      </c>
+      <c r="L58" t="n">
+        <v>40.30569458007812</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.001373767852783203</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>quito intermitente</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>BLK-OFF</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>4</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-0.03164338693022728</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H59" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>67</v>
+      </c>
+      <c r="K59" t="n">
+        <v>5.651785373687744</v>
+      </c>
+      <c r="L59" t="n">
+        <v>-29.83456802368164</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0.001450786599889398</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>recto</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>STR</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>4</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-0.31211918592453</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>82</v>
+      </c>
+      <c r="K60" t="n">
+        <v>6.071146011352539</v>
+      </c>
+      <c r="L60" t="n">
+        <v>-58.08245086669922</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.001885662088170648</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>atención coche</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>CAR-NR</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.07972286641597748</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" t="b">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>32</v>
+      </c>
+      <c r="K61" t="n">
+        <v>-38.62742233276367</v>
+      </c>
+      <c r="L61" t="n">
+        <v>-3.330183744430542</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0.002192325657233596</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>freno</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>B-ON</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.06297258287668228</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H62" t="b">
+        <v>0</v>
+      </c>
+      <c r="I62" t="b">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>26</v>
+      </c>
+      <c r="K62" t="n">
+        <v>-41.75907135009766</v>
+      </c>
+      <c r="L62" t="n">
+        <v>-3.033703565597534</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0.002183513483032584</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>quito intermitente</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>BLK-OFF</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.02244765497744083</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H63" t="b">
+        <v>0</v>
+      </c>
+      <c r="I63" t="b">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>23</v>
+      </c>
+      <c r="K63" t="n">
+        <v>-42.97293853759766</v>
+      </c>
+      <c r="L63" t="n">
+        <v>-2.996037244796753</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0.002199382754042745</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>quito intermitente</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>BLK-OFF</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>4</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-0.800000011920929</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Right_Blinker</t>
+        </is>
+      </c>
+      <c r="H64" t="b">
+        <v>0</v>
+      </c>
+      <c r="I64" t="b">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
+        <v>60</v>
+      </c>
+      <c r="K64" t="n">
+        <v>7.976311683654785</v>
+      </c>
+      <c r="L64" t="n">
+        <v>-24.86974143981934</v>
+      </c>
+      <c r="M64" t="n">
+        <v>0.001613330794498324</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>acelero</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>T-ON</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>4</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.8500000238418579</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-0.1427544355392456</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H65" t="b">
+        <v>0</v>
+      </c>
+      <c r="I65" t="b">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
+        <v>84</v>
+      </c>
+      <c r="K65" t="n">
+        <v>5.431791305541992</v>
+      </c>
+      <c r="L65" t="n">
+        <v>-47.63461303710938</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0.001432781224139035</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>recto</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>STR</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>4</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.1454853415489197</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.01266065053641796</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" t="b">
+        <v>0</v>
+      </c>
+      <c r="J66" t="n">
+        <v>72</v>
+      </c>
+      <c r="K66" t="n">
+        <v>5.094387054443359</v>
+      </c>
+      <c r="L66" t="n">
+        <v>-65.518310546875</v>
+      </c>
+      <c r="M66" t="n">
+        <v>0.002237186301499605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>